<commit_message>
interaktywne dashboardy z użyciem plotly
</commit_message>
<xml_diff>
--- a/pogoda.xlsx
+++ b/pogoda.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1131,6 +1131,44 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>11.81</v>
+      </c>
+      <c r="B19" t="n">
+        <v>11.21</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1019</v>
+      </c>
+      <c r="D19" t="n">
+        <v>83</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>few clouds</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>20</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>18.504</v>
+      </c>
+      <c r="I19" t="n">
+        <v>20</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>19:55:41 02-12-2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>